<commit_message>
add more utility functions, improve error logging
</commit_message>
<xml_diff>
--- a/backend/src/test/resources/templates/excel/imo-crew-list.xlsx
+++ b/backend/src/test/resources/templates/excel/imo-crew-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte.schwitters/Projects/privat/eventplanner/backend/src/main/resources/templates/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte.schwitters/Projects/privat/eventplanner/backend/src/test/resources/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E583C6EE-BA4B-0B4D-B83D-64A562415229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FD3F92-CFD0-3140-8920-F3D52602F117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IMO Crewliste" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="26">
   <si>
     <t>IMO CREW LIST</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>1. Name of ship</t>
-  </si>
-  <si>
-    <t>Grossherzogin Elisabeth / DGEN</t>
   </si>
   <si>
     <t>4. Nationality of ship</t>
@@ -69,9 +66,6 @@
   </si>
   <si>
     <t>11. Date and place of birth</t>
-  </si>
-  <si>
-    <t>German</t>
   </si>
   <si>
     <t>11. Nature and No. of identity document</t>
@@ -640,6 +634,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -647,27 +662,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1012,7 +1006,7 @@
   <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1045,7 +1039,7 @@
     </row>
     <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1068,13 +1062,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="7">
@@ -1089,43 +1083,41 @@
       <c r="C4" s="31"/>
       <c r="D4" s="32"/>
       <c r="E4" s="33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
       <c r="I4" s="35"/>
       <c r="J4" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="36"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
       <c r="D5" s="38"/>
       <c r="E5" s="39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="40"/>
       <c r="G5" s="40"/>
       <c r="H5" s="40"/>
       <c r="I5" s="41"/>
       <c r="J5" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
       <c r="D6" s="32"/>
       <c r="E6" s="33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -1134,9 +1126,7 @@
       <c r="J6" s="42"/>
     </row>
     <row r="7" spans="1:10" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="36"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
       <c r="D7" s="38"/>
@@ -1149,26 +1139,26 @@
     </row>
     <row r="8" spans="1:10" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="24" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1176,27 +1166,27 @@
         <v>1</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="F9" s="25"/>
+      <c r="G9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="H9" s="25"/>
+      <c r="I9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="27" t="s">
+      <c r="J9" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1205,27 +1195,27 @@
         <v>2</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="28"/>
       <c r="I10" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1234,27 +1224,27 @@
         <v>3</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="28"/>
       <c r="I11" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1263,27 +1253,27 @@
         <v>4</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="28"/>
       <c r="I12" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1292,27 +1282,27 @@
         <v>5</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="28"/>
       <c r="I13" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1321,27 +1311,27 @@
         <v>6</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="28"/>
       <c r="I14" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1350,27 +1340,27 @@
         <v>7</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="28"/>
       <c r="I15" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1379,27 +1369,27 @@
         <v>8</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="28"/>
       <c r="I16" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1408,27 +1398,27 @@
         <v>9</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="27"/>
+      <c r="G17" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="28"/>
       <c r="I17" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1437,27 +1427,27 @@
         <v>10</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="27"/>
+      <c r="G18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="28"/>
       <c r="I18" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1466,27 +1456,27 @@
         <v>11</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="28"/>
       <c r="I19" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1495,27 +1485,27 @@
         <v>12</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="28"/>
       <c r="I20" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1524,27 +1514,27 @@
         <v>13</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="27"/>
+      <c r="G21" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="28"/>
       <c r="I21" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1553,27 +1543,27 @@
         <v>14</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="28"/>
       <c r="I22" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,27 +1572,27 @@
         <v>15</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="28"/>
       <c r="I23" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1611,27 +1601,27 @@
         <v>16</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="28"/>
       <c r="I24" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1640,27 +1630,27 @@
         <v>17</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="28"/>
       <c r="I25" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1669,27 +1659,27 @@
         <v>18</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="28"/>
       <c r="I26" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1698,27 +1688,27 @@
         <v>19</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="28"/>
       <c r="I27" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1727,27 +1717,27 @@
         <v>20</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="28"/>
       <c r="I28" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1756,27 +1746,27 @@
         <v>21</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="27"/>
+      <c r="G29" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="28"/>
       <c r="I29" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1785,27 +1775,27 @@
         <v>22</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="28"/>
       <c r="I30" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1814,27 +1804,27 @@
         <v>23</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="G31" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="28"/>
       <c r="I31" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1843,27 +1833,27 @@
         <v>24</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="27"/>
+      <c r="G32" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="28"/>
       <c r="I32" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1872,27 +1862,27 @@
         <v>25</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="27"/>
+      <c r="G33" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="28"/>
       <c r="I33" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1901,27 +1891,27 @@
         <v>26</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="27"/>
+      <c r="G34" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="28"/>
       <c r="I34" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1930,27 +1920,27 @@
         <v>27</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="27"/>
+      <c r="G35" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="28"/>
       <c r="I35" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,27 +1949,27 @@
         <v>28</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="27"/>
+      <c r="G36" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="28"/>
       <c r="I36" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1988,27 +1978,27 @@
         <v>29</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="27"/>
+      <c r="G37" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="28"/>
       <c r="I37" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2017,27 +2007,27 @@
         <v>30</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="20"/>
-      <c r="G38" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="27"/>
+      <c r="G38" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="28"/>
       <c r="I38" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2046,27 +2036,27 @@
         <v>31</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="28"/>
       <c r="I39" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J39" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2075,27 +2065,27 @@
         <v>32</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="20"/>
-      <c r="G40" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H40" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="27"/>
+      <c r="G40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="28"/>
       <c r="I40" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J40" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2104,27 +2094,27 @@
         <v>33</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="27"/>
+      <c r="G41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="28"/>
       <c r="I41" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J41" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2133,27 +2123,27 @@
         <v>34</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="27"/>
+      <c r="G42" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="28"/>
       <c r="I42" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J42" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2162,27 +2152,27 @@
         <v>35</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="27"/>
+      <c r="G43" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="28"/>
       <c r="I43" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J43" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2191,27 +2181,27 @@
         <v>36</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H44" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="27"/>
+      <c r="G44" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="28"/>
       <c r="I44" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J44" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2220,27 +2210,27 @@
         <v>37</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="27"/>
+      <c r="G45" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="28"/>
       <c r="I45" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J45" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2249,27 +2239,27 @@
         <v>38</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H46" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="27"/>
+      <c r="G46" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="28"/>
       <c r="I46" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J46" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2278,27 +2268,27 @@
         <v>39</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="27"/>
+      <c r="G47" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="28"/>
       <c r="I47" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J47" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2307,27 +2297,27 @@
         <v>40</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H48" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="27"/>
+      <c r="G48" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="28"/>
       <c r="I48" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2336,27 +2326,27 @@
         <v>41</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H49" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="27"/>
+      <c r="G49" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="28"/>
       <c r="I49" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2365,27 +2355,27 @@
         <v>42</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H50" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="27"/>
+      <c r="G50" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="28"/>
       <c r="I50" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2394,27 +2384,27 @@
         <v>43</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H51" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="27"/>
+      <c r="G51" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="28"/>
       <c r="I51" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J51" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2423,27 +2413,27 @@
         <v>44</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="20"/>
-      <c r="G52" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H52" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="27"/>
+      <c r="G52" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="28"/>
       <c r="I52" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J52" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2452,27 +2442,27 @@
         <v>45</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="27"/>
+      <c r="G53" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="28"/>
       <c r="I53" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J53" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2481,27 +2471,27 @@
         <v>46</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F54" s="20"/>
-      <c r="G54" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H54" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="27"/>
+      <c r="G54" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="28"/>
       <c r="I54" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J54" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2510,27 +2500,27 @@
         <v>47</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F55" s="20"/>
-      <c r="G55" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H55" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="27"/>
+      <c r="G55" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="28"/>
       <c r="I55" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J55" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2539,27 +2529,27 @@
         <v>48</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F56" s="20"/>
-      <c r="G56" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H56" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="27"/>
+      <c r="G56" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="28"/>
       <c r="I56" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J56" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2568,27 +2558,27 @@
         <v>49</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H57" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="27"/>
+      <c r="G57" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="28"/>
       <c r="I57" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J57" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2597,27 +2587,27 @@
         <v>50</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" s="20"/>
-      <c r="G58" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H58" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="27"/>
+      <c r="G58" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="28"/>
       <c r="I58" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J58" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2626,27 +2616,27 @@
         <v>51</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="20"/>
-      <c r="G59" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H59" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="27"/>
+      <c r="G59" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="28"/>
       <c r="I59" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J59" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2655,27 +2645,27 @@
         <v>52</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H60" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="27"/>
+      <c r="G60" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="28"/>
       <c r="I60" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J60" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2684,27 +2674,27 @@
         <v>53</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F61" s="20"/>
-      <c r="G61" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H61" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="27"/>
+      <c r="G61" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="28"/>
       <c r="I61" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J61" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2713,27 +2703,27 @@
         <v>54</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E62" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H62" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="27"/>
+      <c r="G62" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="28"/>
       <c r="I62" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J62" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2742,27 +2732,27 @@
         <v>55</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="20"/>
-      <c r="G63" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H63" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="27"/>
+      <c r="G63" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="28"/>
       <c r="I63" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J63" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2771,27 +2761,27 @@
         <v>56</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="20"/>
-      <c r="G64" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H64" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="27"/>
+      <c r="G64" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="28"/>
       <c r="I64" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J64" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2800,27 +2790,27 @@
         <v>57</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" s="20"/>
-      <c r="G65" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H65" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="27"/>
+      <c r="G65" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="28"/>
       <c r="I65" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J65" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2829,27 +2819,27 @@
         <v>58</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F66" s="20"/>
-      <c r="G66" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H66" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="27"/>
+      <c r="G66" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" s="28"/>
       <c r="I66" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J66" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2858,27 +2848,27 @@
         <v>59</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H67" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" s="27"/>
+      <c r="G67" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" s="28"/>
       <c r="I67" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J67" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2887,27 +2877,27 @@
         <v>60</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F68" s="20"/>
-      <c r="G68" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H68" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E68" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" s="27"/>
+      <c r="G68" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" s="28"/>
       <c r="I68" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J68" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2916,27 +2906,27 @@
         <v>61</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F69" s="20"/>
-      <c r="G69" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H69" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E69" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" s="27"/>
+      <c r="G69" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" s="28"/>
       <c r="I69" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J69" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2945,27 +2935,27 @@
         <v>62</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70" s="20"/>
-      <c r="G70" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H70" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" s="27"/>
+      <c r="G70" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70" s="28"/>
       <c r="I70" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J70" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2974,27 +2964,27 @@
         <v>63</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F71" s="20"/>
-      <c r="G71" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H71" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" s="27"/>
+      <c r="G71" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="28"/>
       <c r="I71" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J71" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -3003,27 +2993,27 @@
         <v>64</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F72" s="20"/>
-      <c r="G72" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H72" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="27"/>
+      <c r="G72" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="28"/>
       <c r="I72" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J72" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -3032,56 +3022,56 @@
         <v>65</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E73" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F73" s="20"/>
-      <c r="G73" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H73" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E73" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" s="27"/>
+      <c r="G73" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="28"/>
       <c r="I73" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J73" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
-        <f t="shared" ref="A74:A105" si="2">IF(B74 &lt;&gt; "", A73+1, "")</f>
+        <f t="shared" ref="A74:A75" si="2">IF(B74 &lt;&gt; "", A73+1, "")</f>
         <v>66</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F74" s="20"/>
-      <c r="G74" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H74" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E74" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" s="27"/>
+      <c r="G74" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="28"/>
       <c r="I74" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J74" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -3090,31 +3080,161 @@
         <v>67</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F75" s="20"/>
-      <c r="G75" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H75" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="E75" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" s="27"/>
+      <c r="G75" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="28"/>
       <c r="I75" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J75" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="147">
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:I8"/>
@@ -3132,136 +3252,6 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="G73:H73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>